<commit_message>
added new css in html file
</commit_message>
<xml_diff>
--- a/employeeemp.xlsx
+++ b/employeeemp.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,6 +550,50 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RE1474</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>swamiraj</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>swami@reposenergy.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RE6472</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>akshay</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>aksh@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>